<commit_message>
Aplicação do CheckList de Gerência - agile_task #2420
Aplicação do CheckList de Gerência - agile_task #2420
</commit_message>
<xml_diff>
--- a/Doc-DD-UFG/Qualidade/Gerência/checklist_de_qualidade_de_processo_e_produto_GPR_MED_GCO_1.0.0_SDD-UFG_201511142200.xlsx
+++ b/Doc-DD-UFG/Qualidade/Gerência/checklist_de_qualidade_de_processo_e_produto_GPR_MED_GCO_1.0.0_SDD-UFG_201511142200.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instruções" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="78">
   <si>
     <t>Instruções de preenchimento do checklist</t>
   </si>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t> Um conjunto adequado de medidas, orientado pelos objetivos de medição, foi identificado e definido?</t>
-  </si>
-  <si>
-    <t>Plano de medição ainda não foi elaborado.</t>
   </si>
   <si>
     <t>Um conjunto adequado de medidas, orientado pelos objetivos de medição, foi documentado e revisado?</t>
@@ -503,7 +500,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -638,6 +635,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -783,7 +784,7 @@
   <dimension ref="A1:Z65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="E11 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1494,8 +1495,8 @@
   </sheetPr>
   <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D29" activeCellId="1" sqref="E11 D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3559,8 +3560,8 @@
   </sheetPr>
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3621,12 +3622,12 @@
         <v>56</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="33"/>
+        <v>28</v>
+      </c>
+      <c r="D2" s="33"/>
+      <c r="E2" s="34" t="s">
+        <v>29</v>
+      </c>
       <c r="F2" s="29"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3654,15 +3655,15 @@
         <v>3</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="33"/>
+        <v>28</v>
+      </c>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34" t="s">
+        <v>29</v>
+      </c>
       <c r="F3" s="29"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -3690,15 +3691,15 @@
         <v>4</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="33"/>
+        <v>28</v>
+      </c>
+      <c r="D4" s="33"/>
+      <c r="E4" s="34" t="s">
+        <v>29</v>
+      </c>
       <c r="F4" s="29"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
@@ -3726,15 +3727,15 @@
         <v>5</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="33"/>
+        <v>28</v>
+      </c>
+      <c r="D5" s="33"/>
+      <c r="E5" s="34" t="s">
+        <v>29</v>
+      </c>
       <c r="F5" s="29"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -3762,15 +3763,15 @@
         <v>6</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="33"/>
+        <v>28</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="34" t="s">
+        <v>29</v>
+      </c>
       <c r="F6" s="29"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -3798,15 +3799,15 @@
         <v>7</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="33"/>
+        <v>28</v>
+      </c>
+      <c r="D7" s="33"/>
+      <c r="E7" s="34" t="s">
+        <v>29</v>
+      </c>
       <c r="F7" s="29"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -3834,15 +3835,15 @@
         <v>8</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="33"/>
+        <v>28</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="E8" s="34" t="s">
+        <v>29</v>
+      </c>
       <c r="F8" s="29"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -3873,12 +3874,12 @@
         <v>49</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="33"/>
+        <v>28</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="34" t="s">
+        <v>29</v>
+      </c>
       <c r="F9" s="29"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -3906,15 +3907,15 @@
         <v>10</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="33"/>
+        <v>28</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="34" t="s">
+        <v>29</v>
+      </c>
       <c r="F10" s="29"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
@@ -3945,12 +3946,12 @@
         <v>50</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="33"/>
+        <v>28</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="34" t="s">
+        <v>29</v>
+      </c>
       <c r="F11" s="29"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -3978,15 +3979,15 @@
         <v>12</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="33"/>
+        <v>28</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="34" t="s">
+        <v>29</v>
+      </c>
       <c r="F12" s="29"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
@@ -4014,15 +4015,15 @@
         <v>13</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="33"/>
+        <v>28</v>
+      </c>
+      <c r="D13" s="33"/>
+      <c r="E13" s="34" t="s">
+        <v>29</v>
+      </c>
       <c r="F13" s="29"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -4065,6 +4066,20 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="Exibir"/>
+    <hyperlink ref="E3" r:id="rId2" display="Exibir"/>
+    <hyperlink ref="E4" r:id="rId3" display="Exibir"/>
+    <hyperlink ref="E5" r:id="rId4" display="Exibir"/>
+    <hyperlink ref="E6" r:id="rId5" display="Exibir"/>
+    <hyperlink ref="E7" r:id="rId6" display="Exibir"/>
+    <hyperlink ref="E8" r:id="rId7" display="Exibir"/>
+    <hyperlink ref="E9" r:id="rId8" display="Exibir"/>
+    <hyperlink ref="E10" r:id="rId9" display="Exibir"/>
+    <hyperlink ref="E11" r:id="rId10" display="Exibir"/>
+    <hyperlink ref="E12" r:id="rId11" display="Exibir"/>
+    <hyperlink ref="E13" r:id="rId12" display="Exibir"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4083,7 +4098,7 @@
   <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="E11 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.35"/>
@@ -4105,225 +4120,225 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="37" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37" t="n">
+      <c r="A2" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="40" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="38" t="s">
+      <c r="C3" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="40"/>
+      <c r="E3" s="41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="38" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="38" t="s">
+      <c r="C4" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
+    </row>
+    <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="38" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
-    </row>
-    <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="37" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="38" t="s">
+      <c r="C5" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="D5" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="E5" s="41"/>
+    </row>
+    <row r="6" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="38" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="40"/>
-    </row>
-    <row r="6" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="38" t="s">
+      <c r="C6" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="41"/>
+    </row>
+    <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="38" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C7" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="40"/>
+      <c r="E7" s="41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="38" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="40"/>
+      <c r="E8" s="41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="38" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="40"/>
-    </row>
-    <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="40" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="37" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="40"/>
+      <c r="E9" s="41"/>
     </row>
     <row r="10" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="37" t="n">
+      <c r="A10" s="38" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="40" t="s">
+      <c r="C10" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="40"/>
+      <c r="E10" s="41" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="37" t="n">
+      <c r="A11" s="38" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="40" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="31"/>
-      <c r="E11" s="40"/>
+      <c r="E11" s="41"/>
     </row>
     <row r="12" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="37" t="n">
+      <c r="A12" s="38" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="40"/>
+      <c r="E12" s="41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="38" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="40" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="37" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40" t="s">
+      <c r="C13" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="40"/>
+      <c r="E13" s="41" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="37" t="n">
+      <c r="A14" s="38" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="40" t="s">
+      <c r="C14" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="40"/>
+      <c r="E14" s="41" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="37" t="n">
+      <c r="A15" s="38" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40" t="s">
+      <c r="C15" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="40"/>
+      <c r="E15" s="41" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>